<commit_message>
Fix execution count in notebook and refactor employee summary calculations
</commit_message>
<xml_diff>
--- a/data/2025/case_1/data.xlsx
+++ b/data/2025/case_1/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manugf/projects/planning/data/2025/case_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037633BE-5FD6-344D-9390-F051C0B76E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D166F69-C7FE-D14F-B070-E8F4CA816E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="1160" windowWidth="33160" windowHeight="26380" activeTab="2" xr2:uid="{CE96B702-472C-414A-8924-8EE64351FAC5}"/>
+    <workbookView xWindow="14220" yWindow="1160" windowWidth="33160" windowHeight="26380" activeTab="1" xr2:uid="{CE96B702-472C-414A-8924-8EE64351FAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="01" sheetId="13" r:id="rId1"/>
@@ -5752,8 +5752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD72376-7605-DC48-9DB4-FD6CB4C0C4AF}">
   <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6373,7 +6373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6EE496-D1CB-924B-9DC9-969E4E88A866}">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>